<commit_message>
I really cant spell
</commit_message>
<xml_diff>
--- a/grower_settings.xlsx
+++ b/grower_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bussy\Grower Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DBD624-9F74-45CC-BBA4-93B865ED6713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBECE444-D219-4F71-9B66-435B063C66B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1275" windowWidth="29040" windowHeight="15720" xr2:uid="{BD47AE73-EC2A-4ADF-8E94-B6892A263739}"/>
   </bookViews>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0B725D-3905-44B9-B178-398A0E03EE4D}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>